<commit_message>
dummy data print test
</commit_message>
<xml_diff>
--- a/data/ip_dummy.xlsx
+++ b/data/ip_dummy.xlsx
@@ -21,10 +21,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -68,12 +64,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -355,109 +348,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1">
+        <v>2401</v>
+      </c>
+      <c r="B1">
+        <v>121</v>
+      </c>
+      <c r="C1">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>2402</v>
+      </c>
+      <c r="B2">
+        <v>123</v>
+      </c>
+      <c r="C2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>2403</v>
+      </c>
+      <c r="B3">
+        <v>125</v>
+      </c>
+      <c r="C3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>2404</v>
+      </c>
+      <c r="B4">
+        <v>127</v>
+      </c>
+      <c r="C4">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>2405</v>
+      </c>
+      <c r="B5">
+        <v>129</v>
+      </c>
+      <c r="C5">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6">
         <v>2406</v>
       </c>
-      <c r="B1">
+      <c r="B6">
         <v>131</v>
       </c>
-      <c r="C1">
+      <c r="C6">
         <v>132</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7">
         <v>2407</v>
       </c>
-      <c r="B2">
+      <c r="B7">
         <v>133</v>
       </c>
-      <c r="C2">
+      <c r="C7">
         <v>134</v>
       </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8">
         <v>2408</v>
       </c>
-      <c r="B3">
+      <c r="B8">
         <v>135</v>
       </c>
-      <c r="C3">
+      <c r="C8">
         <v>136</v>
       </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9">
         <v>2409</v>
       </c>
-      <c r="B4">
+      <c r="B9">
         <v>137</v>
       </c>
-      <c r="C4">
+      <c r="C9">
         <v>138</v>
       </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10">
         <v>2410</v>
       </c>
-      <c r="B5">
+      <c r="B10">
         <v>139</v>
       </c>
-      <c r="C5">
+      <c r="C10">
         <v>140</v>
       </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11">
         <v>2411</v>
       </c>
-      <c r="B6">
+      <c r="B11">
         <v>141</v>
       </c>
-      <c r="C6">
+      <c r="C11">
         <v>142</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12">
         <v>2412</v>
       </c>
-      <c r="B7">
+      <c r="B12">
         <v>143</v>
       </c>
-      <c r="C7">
+      <c r="C12">
         <v>144</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13">
         <v>2413</v>
       </c>
-      <c r="B8">
+      <c r="B13">
         <v>145</v>
       </c>
-      <c r="C8">
+      <c r="C13">
         <v>146</v>
       </c>
-      <c r="D8" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>2414</v>
+      </c>
+      <c r="B14">
+        <v>147</v>
+      </c>
+      <c r="C14">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>2415</v>
+      </c>
+      <c r="B15">
+        <v>149</v>
+      </c>
+      <c r="C15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>2416</v>
+      </c>
+      <c r="B16">
+        <v>151</v>
+      </c>
+      <c r="C16">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>2417</v>
+      </c>
+      <c r="B17">
+        <v>153</v>
+      </c>
+      <c r="C17">
+        <v>154</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>